<commit_message>
PCB und BOM Update
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luith\Documents\Projekte\Espressomaschine Upgrades\Espressomaschine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9B6D63-953F-4E99-8133-1B179CCEEF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CB722A-7527-4670-9058-3461D597B67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="1170" windowWidth="16410" windowHeight="20985" xr2:uid="{5295B79B-AABD-4FCC-9474-95C75AE1AA52}"/>
+    <workbookView xWindow="-16305" yWindow="14040" windowWidth="16410" windowHeight="14145" xr2:uid="{5295B79B-AABD-4FCC-9474-95C75AE1AA52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Total" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Mikrocontroller</t>
   </si>
   <si>
-    <t>Thermostat</t>
-  </si>
-  <si>
     <t>https://www.amazon.de/-/en/gp/product/B089B66DX1/ref=ox_sc_act_title_1?smid=A10PGDQ6G32BHL&amp;psc=1</t>
   </si>
   <si>
@@ -114,13 +112,100 @@
   </si>
   <si>
     <t>Montagerolle</t>
+  </si>
+  <si>
+    <t>Wärmeleitpaste</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/gp/product/B0795DP124/ref=sw_img_1?smid=A31522I6NTHR25&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Testing Thermostat</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/mean-well-usa-inc/IRM-05-5/7704652</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/panasonic-electric-works/ALDP105W/3641417</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>nicht sicher</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/diotec-semiconductor/1N4001/13164614</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/onsemi/BC550CBU/975565</t>
+  </si>
+  <si>
+    <t>Power stecker zu Verbaucher</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/keystone-electronics/1287-ST/303577</t>
+  </si>
+  <si>
+    <t>SSR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/w%C3%BCrth-elektronik/691102810001/21764305</t>
+  </si>
+  <si>
+    <t>Schraubanschluss</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/stmicroelectronics/STM32G071CBT6/9749147</t>
+  </si>
+  <si>
+    <t>Dev Board</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/stmicroelectronics/NUCLEO-G071RB/9739925</t>
+  </si>
+  <si>
+    <t>Preis</t>
+  </si>
+  <si>
+    <t>sensorplatine</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/adafruit-industries-llc/270/9565771</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/cantherm/CS704025Y/2195521?srsltid=AfmBOophK-TX-CnZJFt10FCOz_esJuaoXtdsjLbb7I0EY9QXJpteSS7u</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/idec/RSSDN-10A/21445226</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/stmicroelectronics/NUCLEO-G071RB/9739925?s=N4IgTCBcDaIOIAYDsBGASgIRAXQL5A</t>
+  </si>
+  <si>
+    <t>Draht</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/KWOKWEI-Enamelled-Magnetic-Electrical-Engineering/dp/B0DSB7GQMX/ref=sr_1_1_sspa?crid=2LJSUN0AK3IG3&amp;dib=eyJ2IjoiMSJ9.E2yCULG9tgeUGx_a5v2auTokNfhhs9uLr7O6oKQHsYSQNZ43rmMiZCGxJOrOe0UHqF9yn_TMwjsn2AcjwxK5pWW1Yq49jzwmz7gjF_73NjROaIILzpvWGUub1cTzvPk9_nZEh7ic1iGraBjlApCmSyyaPnT379ZLPFuOFMWe1tHOVOwZj_EKIfI-uFYbUDhW_Rv2Md2jHfnqfv498WZLVWICsIZuBgRpHxXZV9cjXdcobK1mEwVbBitMMNxphSY92VH_bj5EzS_NKtm6OHqSNoYdL-B8AefDculBOnvLXp8.qrEHQLldfADOyPcGwz8EZesS_ydCpTfuQweDSaPD5jw&amp;dib_tag=se&amp;keywords=kupferlackdraht%2B1%2C5mm&amp;qid=1763246254&amp;sprefix=kupferlackdraht%2B1%2Caps%2C96&amp;sr=8-1-spons&amp;aref=p7F8CA0lUS&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +221,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -213,11 +312,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -226,8 +341,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7B8830-9ED1-4F88-AADE-BA7CA5F110EB}">
-  <dimension ref="B1:E21"/>
+  <dimension ref="B1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,10 +702,11 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,11 +714,14 @@
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -595,129 +729,536 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D26" r:id="rId1" xr:uid="{0B325DB1-71A3-4DE2-A7AE-660B2DC66AD7}"/>
+    <hyperlink ref="D33" r:id="rId2" xr:uid="{8BF15B32-4C1F-4962-9E28-BCB222B34FF0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02593D75-B579-406F-815C-26529303AF29}">
+  <dimension ref="B1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <f>E4*8.59</f>
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <f>E9*0.86</f>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10">
+        <f>E10*0.88</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <f>E11*0.11</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <f>E12*0.25</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5">
+        <v>5</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <f>E13*0.15</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14">
+        <f>E14*28.47</f>
+        <v>56.94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15">
+        <f>E15*9.54</f>
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16">
+        <v>16.989999999999998</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{84E1A967-9580-41F2-9208-60D2B50F464F}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{69DB1854-B6DA-4FCC-A5BD-73C589745965}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>